<commit_message>
removed duplicate in his data
</commit_message>
<xml_diff>
--- a/data/his/original_data/his_APC_Sweden_201701-201810.xlsx
+++ b/data/his/original_data/his_APC_Sweden_201701-201810.xlsx
@@ -297,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="1" shapeId="0">
+    <comment ref="C18" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -317,11 +317,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Via SEK (40% discount)</t>
+Via SEK</t>
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="1" shapeId="0">
+    <comment ref="C26" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -393,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C29" authorId="1" shapeId="0">
+    <comment ref="C31" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -413,35 +413,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Via SEK</t>
+Converted 2018-11-30</t>
         </r>
       </text>
     </comment>
     <comment ref="C32" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qiuhong Boers:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Converted 2018-11-30</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C33" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -492,7 +468,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="125">
   <si>
     <t>institution</t>
   </si>
@@ -1056,7 +1032,18 @@
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1336,28 +1323,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.4140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +1379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>124</v>
       </c>
@@ -1423,7 +1410,7 @@
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>124</v>
       </c>
@@ -1456,7 +1443,7 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>124</v>
       </c>
@@ -1487,7 +1474,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>124</v>
       </c>
@@ -1518,7 +1505,7 @@
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>124</v>
       </c>
@@ -1549,7 +1536,7 @@
       </c>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>124</v>
       </c>
@@ -1580,7 +1567,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>124</v>
       </c>
@@ -1611,7 +1598,7 @@
       </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>124</v>
       </c>
@@ -1644,7 +1631,7 @@
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>124</v>
       </c>
@@ -1677,7 +1664,7 @@
       </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>124</v>
       </c>
@@ -1710,7 +1697,7 @@
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>124</v>
       </c>
@@ -1743,7 +1730,7 @@
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>124</v>
       </c>
@@ -1776,7 +1763,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>124</v>
       </c>
@@ -1784,7 +1771,7 @@
         <v>2017</v>
       </c>
       <c r="C14" s="3">
-        <v>885</v>
+        <v>1335</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>58</v>
@@ -1807,82 +1794,84 @@
       <c r="J14" s="13"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B15" s="18">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C15" s="6">
-        <v>450</v>
+        <v>1590.7</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>61</v>
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="13"/>
+        <v>63</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B16" s="18">
         <v>2018</v>
       </c>
-      <c r="C16" s="6">
-        <v>1590.7</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>65</v>
+      <c r="C16" s="3">
+        <v>2651.16</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E16" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="4" t="s">
         <v>66</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B17" s="18">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C17" s="3">
-        <v>2651.16</v>
+        <v>1937.65</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E17" s="3" t="b">
         <v>1</v>
@@ -1891,84 +1880,82 @@
         <v>66</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B18" s="18">
+        <v>2018</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1328.5170000000001</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="18">
         <v>2017</v>
       </c>
-      <c r="C18" s="3">
-        <v>1937.65</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="18">
-        <v>2018</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1328.5170000000001</v>
+      <c r="C19" s="3">
+        <v>1305</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>78</v>
+      <c r="F19" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>124</v>
       </c>
@@ -1979,13 +1966,13 @@
         <v>1305</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>13</v>
@@ -1999,49 +1986,51 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B21" s="18">
+        <v>2018</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2083</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="18">
         <v>2017</v>
       </c>
-      <c r="C21" s="3">
-        <v>1305</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22" s="18">
-        <v>2018</v>
-      </c>
       <c r="C22" s="3">
-        <v>2083</v>
+        <v>2500</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>1</v>
@@ -2050,31 +2039,31 @@
         <v>91</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B23" s="18">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C23" s="3">
-        <v>2500</v>
+        <v>2083</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>1</v>
@@ -2083,20 +2072,20 @@
         <v>91</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>124</v>
       </c>
@@ -2104,32 +2093,32 @@
         <v>2018</v>
       </c>
       <c r="C24" s="3">
-        <v>2083</v>
+        <v>1500</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>124</v>
       </c>
@@ -2137,65 +2126,63 @@
         <v>2018</v>
       </c>
       <c r="C25" s="3">
-        <v>1500</v>
+        <v>608</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E25" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B26" s="18">
-        <v>2018</v>
-      </c>
-      <c r="C26" s="3">
-        <v>608</v>
+        <v>2017</v>
+      </c>
+      <c r="C26" s="6">
+        <v>2276.7600000000002</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>123</v>
+        <v>29</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>101</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="I26" s="16"/>
       <c r="J26" s="16" t="s">
-        <v>102</v>
+        <v>30</v>
       </c>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>124</v>
       </c>
@@ -2203,30 +2190,30 @@
         <v>2017</v>
       </c>
       <c r="C27" s="6">
-        <v>2276.7600000000002</v>
+        <v>1271.6600000000001</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E27" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>106</v>
+      <c r="F27" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="16" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>124</v>
       </c>
@@ -2234,10 +2221,10 @@
         <v>2017</v>
       </c>
       <c r="C28" s="6">
-        <v>1271.6600000000001</v>
+        <v>1318.47</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>0</v>
@@ -2257,7 +2244,7 @@
       </c>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>124</v>
       </c>
@@ -2265,30 +2252,32 @@
         <v>2017</v>
       </c>
       <c r="C29" s="6">
-        <v>1318.47</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>108</v>
+        <v>630</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="E29" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I29" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>120</v>
+      </c>
       <c r="J29" s="16" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>124</v>
       </c>
@@ -2296,116 +2285,86 @@
         <v>2017</v>
       </c>
       <c r="C30" s="6">
-        <v>630</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>109</v>
+        <v>1539.9</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="E30" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>120</v>
+      <c r="F30" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B31" s="18">
         <v>2017</v>
       </c>
-      <c r="C31" s="6">
-        <v>1539.9</v>
+      <c r="C31" s="3">
+        <v>1817.42</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="I31" s="16" t="s">
-        <v>113</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="I31" s="16"/>
       <c r="J31" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B32" s="18">
-        <v>2017</v>
-      </c>
-      <c r="C32" s="3">
-        <v>1817.42</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E32" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="H32" s="16" t="s">
         <v>119</v>
       </c>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="6"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="17"/>
       <c r="I32" s="16"/>
-      <c r="J32" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="6"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="3"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="F36" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B39" s="11"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="14"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="11"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.19080/OAJT.2018.02.555597"/>
     <hyperlink ref="D5" r:id="rId2" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.12688/f1000research.12418.2"/>
@@ -2417,23 +2376,23 @@
     <hyperlink ref="D11" r:id="rId8" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1073/pnas.1800727115"/>
     <hyperlink ref="D12" r:id="rId9" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1177/1476750317723965"/>
     <hyperlink ref="D13" r:id="rId10" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1155/2018/9618036"/>
-    <hyperlink ref="D17" r:id="rId11" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1016/j.srhc.2018.07.001"/>
-    <hyperlink ref="D18" r:id="rId12" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1016/j.orhc.2017.10.003"/>
-    <hyperlink ref="D19" r:id="rId13" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1371/journal.pone.0200329"/>
-    <hyperlink ref="D20" r:id="rId14" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1038/s41598-017-11204-1"/>
-    <hyperlink ref="D21" r:id="rId15" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1038/s41598-017-16174-y"/>
-    <hyperlink ref="D22" r:id="rId16" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1002/int.22034"/>
-    <hyperlink ref="D23" r:id="rId17" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1111/ijn.12603"/>
-    <hyperlink ref="D24" r:id="rId18" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1111/1468-5973.12230"/>
-    <hyperlink ref="D25" r:id="rId19" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1002/stem.2908"/>
-    <hyperlink ref="D26" r:id="rId20" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1007/978-3-319-99771-1_22"/>
-    <hyperlink ref="D27" r:id="rId21" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.3389/fpsyg.2017.00036"/>
-    <hyperlink ref="D28" r:id="rId22" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1371/journal.pone.0179613"/>
-    <hyperlink ref="D29" r:id="rId23" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1371/journal.pone.0170613"/>
-    <hyperlink ref="F31" r:id="rId24" display="http://www.elsevier.com/"/>
-    <hyperlink ref="G31" r:id="rId25" display="http://www.elsevier.com/wps/product/cws_home/622931/description"/>
-    <hyperlink ref="D31" r:id="rId26" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1016/j.phrs.2017.10.012"/>
-    <hyperlink ref="D32" r:id="rId27" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1186/s12884-017-1411-8"/>
+    <hyperlink ref="D16" r:id="rId11" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1016/j.srhc.2018.07.001"/>
+    <hyperlink ref="D17" r:id="rId12" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1016/j.orhc.2017.10.003"/>
+    <hyperlink ref="D18" r:id="rId13" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1371/journal.pone.0200329"/>
+    <hyperlink ref="D19" r:id="rId14" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1038/s41598-017-11204-1"/>
+    <hyperlink ref="D20" r:id="rId15" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1038/s41598-017-16174-y"/>
+    <hyperlink ref="D21" r:id="rId16" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1002/int.22034"/>
+    <hyperlink ref="D22" r:id="rId17" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1111/ijn.12603"/>
+    <hyperlink ref="D23" r:id="rId18" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1111/1468-5973.12230"/>
+    <hyperlink ref="D24" r:id="rId19" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1002/stem.2908"/>
+    <hyperlink ref="D25" r:id="rId20" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1007/978-3-319-99771-1_22"/>
+    <hyperlink ref="D26" r:id="rId21" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.3389/fpsyg.2017.00036"/>
+    <hyperlink ref="D27" r:id="rId22" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1371/journal.pone.0179613"/>
+    <hyperlink ref="D28" r:id="rId23" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1371/journal.pone.0170613"/>
+    <hyperlink ref="F30" r:id="rId24" display="http://www.elsevier.com/"/>
+    <hyperlink ref="G30" r:id="rId25" display="http://www.elsevier.com/wps/product/cws_home/622931/description"/>
+    <hyperlink ref="D30" r:id="rId26" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1016/j.phrs.2017.10.012"/>
+    <hyperlink ref="D31" r:id="rId27" tooltip="Länk till fulltext i originalpublikationen. Kräver vanligen prenumeration för åtkomst." display="https://doi.org/10.1186/s12884-017-1411-8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>

</xml_diff>